<commit_message>
processing 0.5.0 up to Collections
</commit_message>
<xml_diff>
--- a/templates/VocExcel-template_050.xlsx
+++ b/templates/VocExcel-template_050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/rdflib/VocExcel/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9277F59A-54E4-964F-8AAB-9BC2322DA457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D468E598-1A87-2144-B3F9-542E46CCF179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="112">
   <si>
     <t>Version:</t>
   </si>
@@ -165,12 +165,6 @@
     <t>Collections</t>
   </si>
   <si>
-    <t>Preferred Label</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
     <t>Prefix</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
   </si>
   <si>
     <t>Optional: an IRI if you have one, else just a name</t>
-  </si>
-  <si>
-    <t>Collection IRI</t>
   </si>
   <si>
     <t>0.5.0</t>
@@ -595,9 +586,6 @@
     <t>An optional statement about the origin of this Concept</t>
   </si>
   <si>
-    <t>Soure</t>
-  </si>
-  <si>
     <t>An optional hyperlink to source information</t>
   </si>
   <si>
@@ -605,10 +593,6 @@
   </si>
   <si>
     <t>The Concept IRIs of any Concepts that are children of this one. The IRIs must be present in Column A.
-Separated by a newline or comma.</t>
-  </si>
-  <si>
-    <t>Alternate labels.
 Separated by a newline or comma.</t>
   </si>
   <si>
@@ -725,9 +709,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Members IRIs</t>
-  </si>
-  <si>
     <t>Definition/description of this vocabulary</t>
   </si>
   <si>
@@ -750,6 +731,22 @@
   </si>
   <si>
     <t>IRI for this vocabulary. See the Documentation Sheet's IRI section</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Concept IRI*</t>
+  </si>
+  <si>
+    <t>Alternate labels, optional.
+Separated by a newline or comma.</t>
+  </si>
+  <si>
+    <t>Collection IRI*</t>
+  </si>
+  <si>
+    <t>Members IRIs*</t>
   </si>
 </sst>
 </file>
@@ -1109,14 +1106,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1188,12 +1179,6 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1208,12 +1193,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1232,13 +1211,31 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1491,26 +1488,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="28"/>
-    <col min="2" max="2" width="59.83203125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="28"/>
-    <col min="4" max="4" width="24" style="30" customWidth="1"/>
-    <col min="5" max="9" width="12.5" style="28"/>
-    <col min="10" max="10" width="21.33203125" style="28" customWidth="1"/>
-    <col min="11" max="24" width="12.5" style="28"/>
-    <col min="25" max="25" width="12.5" style="28" customWidth="1"/>
-    <col min="26" max="26" width="9.6640625" style="28" customWidth="1"/>
-    <col min="27" max="16384" width="12.5" style="28"/>
+    <col min="1" max="1" width="12.5" style="27"/>
+    <col min="2" max="2" width="59.83203125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="27"/>
+    <col min="4" max="4" width="24" style="28" customWidth="1"/>
+    <col min="5" max="9" width="12.5" style="27"/>
+    <col min="10" max="10" width="21.33203125" style="27" customWidth="1"/>
+    <col min="11" max="24" width="12.5" style="27"/>
+    <col min="25" max="25" width="12.5" style="27" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" style="27" customWidth="1"/>
+    <col min="27" max="16384" width="12.5" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="26"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1518,12 +1515,12 @@
     </row>
     <row r="2" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="26"/>
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
@@ -1541,97 +1538,97 @@
     </row>
     <row r="4" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="6" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="31" t="s">
-        <v>36</v>
+      <c r="B8" s="29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.15"/>
     <row r="10" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="11" spans="1:11" ht="28" x14ac:dyDescent="0.15">
-      <c r="B11" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="32" t="s">
+      <c r="B11" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>35</v>
+      <c r="E11" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="D12" s="28"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.15">
-      <c r="B13" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="32" t="s">
+      <c r="B13" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="34" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="B14" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:11" ht="28" x14ac:dyDescent="0.15">
+      <c r="B15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="B16" s="33"/>
+    </row>
+    <row r="17" spans="2:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="27"/>
+    </row>
+    <row r="20" spans="2:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
-      <c r="B14" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:11" ht="28" x14ac:dyDescent="0.15">
-      <c r="B15" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="35"/>
-    </row>
-    <row r="17" spans="2:5" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="27"/>
     </row>
     <row r="21" spans="2:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="D21" s="28"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="2:5" ht="13" x14ac:dyDescent="0.15"/>
     <row r="23" spans="2:5" ht="13" x14ac:dyDescent="0.15"/>
@@ -2639,7 +2636,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27" style="36" customWidth="1"/>
+    <col min="1" max="1" width="27" style="34" customWidth="1"/>
     <col min="2" max="2" width="108.33203125" style="18" customWidth="1"/>
     <col min="3" max="3" width="60" style="20" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="18"/>
@@ -2647,61 +2644,61 @@
   <sheetData>
     <row r="2" spans="1:3" ht="63" x14ac:dyDescent="0.15">
       <c r="B2" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="209" x14ac:dyDescent="0.15">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="364" x14ac:dyDescent="0.15">
+      <c r="A4" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="364" x14ac:dyDescent="0.15">
-      <c r="A4" s="36" t="s">
+      <c r="C4" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="211" x14ac:dyDescent="0.15">
+      <c r="A5" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="97" x14ac:dyDescent="0.15">
+      <c r="A6" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.15">
+      <c r="A7" s="35"/>
+      <c r="B7" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="211" x14ac:dyDescent="0.15">
-      <c r="A5" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="97" x14ac:dyDescent="0.15">
-      <c r="A6" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="25"/>
-    </row>
-    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
-      <c r="B7" s="24" t="s">
-        <v>52</v>
-      </c>
       <c r="C7" s="22"/>
     </row>
     <row r="8" spans="1:3" ht="38" x14ac:dyDescent="0.15">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="17"/>
     </row>
@@ -2710,11 +2707,11 @@
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="76" x14ac:dyDescent="0.15">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="18"/>
     </row>
@@ -2723,11 +2720,11 @@
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A12" s="36" t="s">
-        <v>47</v>
+      <c r="A12" s="34" t="s">
+        <v>44</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="17"/>
     </row>
@@ -2736,11 +2733,11 @@
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" ht="38" x14ac:dyDescent="0.15">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="34" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="17"/>
     </row>
@@ -2749,11 +2746,11 @@
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.15">
-      <c r="A16" s="36" t="s">
-        <v>46</v>
+      <c r="A16" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C16" s="17"/>
     </row>
@@ -2773,8 +2770,8 @@
   </sheetPr>
   <dimension ref="A1:D998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2786,131 +2783,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="C2" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="58" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="64" t="s">
+    <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A10" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="64" t="s">
+      <c r="D11" s="58" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A10" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="64" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5890,126 +5887,126 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="49.1640625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.5" style="43" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" style="43" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="42"/>
+    <col min="1" max="1" width="49.1640625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.5" style="41" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="41" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.15">
-      <c r="A2" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="57" t="s">
+      <c r="A2" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="133" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="57" t="s">
+      <c r="D4" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="57" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="133" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="F4" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="95" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="43" t="s">
+      <c r="C5" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="76" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="95" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="42" t="s">
+      <c r="C6" s="38" t="s">
         <v>78</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="76" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -6040,84 +6037,84 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.5" style="66" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" style="60" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="25.1640625" style="10" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" style="10" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="A1" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:27" s="39" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+    <row r="2" spans="1:27" s="37" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="F2" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="69" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="67" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="71" t="s">
-        <v>111</v>
-      </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65"/>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
+      <c r="G2" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="61" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A3" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
     </row>
     <row r="4" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I4" s="3"/>
@@ -6155,15 +6152,15 @@
   </sheetPr>
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="34" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="47.83203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="45.5" style="6" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="6" customWidth="1"/>
@@ -6171,28 +6168,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="60" t="s">
+      <c r="A2" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="56" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="5"/>
@@ -7639,62 +7636,62 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="12.5" style="28"/>
+    <col min="1" max="1" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="12.5" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="73" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.15">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="43"/>
+    </row>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+      <c r="A3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="45"/>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.15">
-      <c r="A3" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.15">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+    </row>
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+      <c r="A5" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-    </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.15">
-      <c r="A5" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>